<commit_message>
Added Dictionary backend and integration with Riot Data Dragon
</commit_message>
<xml_diff>
--- a/Version_1/LearningScripts/Raw Excel Output of Match+Info.xlsx
+++ b/Version_1/LearningScripts/Raw Excel Output of Match+Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OKsho\Desktop\repos\RiotAPIProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OKsho\Desktop\repos\LOLBreakdown\Version_1\LearningScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669FFF0C-6896-4D19-AF1F-9A7B6EBED16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802BADF3-B6AA-4D50-B481-CF168C7D06FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -180,10 +180,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,32 +488,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -580,7 +580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>